<commit_message>
el programa funciona correctamente
</commit_message>
<xml_diff>
--- a/src/utilitarios/FACTORES DE CONVERSION.xlsx
+++ b/src/utilitarios/FACTORES DE CONVERSION.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ARCHIVOS DE CURSOS ALURA\11 ESPECIALIZACION JAVA BACK-END\WORKSPACE_ALURA\Challenge-Oracle-One-Conversor-De-Monedas\src\utilitarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8F65B0-BB6A-457E-BFC5-C92B000309A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD470474-D162-4AAE-BE97-901A18AC2F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="4" xr2:uid="{265E011E-F8F9-431A-9CD5-1A57F952F6C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{265E011E-F8F9-431A-9CD5-1A57F952F6C2}"/>
   </bookViews>
   <sheets>
-    <sheet name="DIVISAS" sheetId="5" r:id="rId1"/>
-    <sheet name="LONGITUDES" sheetId="4" r:id="rId2"/>
-    <sheet name="MASAS" sheetId="1" r:id="rId3"/>
-    <sheet name="VELOCIDADES" sheetId="2" r:id="rId4"/>
-    <sheet name="VOLUMENES" sheetId="3" r:id="rId5"/>
+    <sheet name="TEMPERATURAS" sheetId="6" r:id="rId1"/>
+    <sheet name="DIVISAS" sheetId="5" r:id="rId2"/>
+    <sheet name="LONGITUDES" sheetId="4" r:id="rId3"/>
+    <sheet name="MASAS" sheetId="1" r:id="rId4"/>
+    <sheet name="VELOCIDADES" sheetId="2" r:id="rId5"/>
+    <sheet name="VOLUMENES" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>SIMBOLOS</t>
   </si>
@@ -317,6 +318,24 @@
   </si>
   <si>
     <t>JPY-&gt;SVC</t>
+  </si>
+  <si>
+    <t>C-&gt;F</t>
+  </si>
+  <si>
+    <t>F-&gt;C</t>
+  </si>
+  <si>
+    <t>C-&gt;K</t>
+  </si>
+  <si>
+    <t>F-&gt;K</t>
+  </si>
+  <si>
+    <t>K-&gt;C</t>
+  </si>
+  <si>
+    <t>K-&gt;F</t>
   </si>
 </sst>
 </file>
@@ -707,6 +726,112 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D944A52-4B3D-487B-9957-1D7446C57E10}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="55.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"rates.put("""&amp;A2&amp;""",new BigDecimal("""&amp;B2&amp;"""));"</f>
+        <v>rates.put("C-&gt;F",new BigDecimal("1"));</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <f>"rates.put("""&amp;A3&amp;""",new BigDecimal("""&amp;B3&amp;"""));"</f>
+        <v>rates.put("C-&gt;K",new BigDecimal("1"));</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <f>"rates.put("""&amp;A4&amp;""",new BigDecimal("""&amp;B4&amp;"""));"</f>
+        <v>rates.put("F-&gt;C",new BigDecimal("1"));</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <f>"rates.put("""&amp;A5&amp;""",new BigDecimal("""&amp;B5&amp;"""));"</f>
+        <v>rates.put("F-&gt;K",new BigDecimal("1"));</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <f>"rates.put("""&amp;A6&amp;""",new BigDecimal("""&amp;B6&amp;"""));"</f>
+        <v>rates.put("K-&gt;C",new BigDecimal("1"));</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <f>"rates.put("""&amp;A7&amp;""",new BigDecimal("""&amp;B7&amp;"""));"</f>
+        <v>rates.put("K-&gt;F",new BigDecimal("1"));</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C7">
+    <sortCondition ref="A2:A7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E240AFEF-D292-48AE-B5D3-4E0CF016EAC5}">
   <dimension ref="A1:C31"/>
   <sheetViews>
@@ -1095,7 +1220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E108E094-89F6-4FE9-99C6-43F392D88A17}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1270,7 +1395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{467F7111-EF0D-4B7E-853A-7943D033F7D1}">
   <dimension ref="A1:C31"/>
   <sheetViews>
@@ -1665,7 +1790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCADF1FD-7F1E-4886-A1DF-216AA75223B9}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1770,11 +1895,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D6EA872-F9A9-49EC-B352-1DBF2D7BF593}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1804,7 +1929,7 @@
         <v>0.1</v>
       </c>
       <c r="C2" t="str">
-        <f>"rates.put("""&amp;A2&amp;""",new BigDecimal("""&amp;B2&amp;"""));"</f>
+        <f t="shared" ref="C2:C13" si="0">"rates.put("""&amp;A2&amp;""",new BigDecimal("""&amp;B2&amp;"""));"</f>
         <v>rates.put("cm-&gt;dm",new BigDecimal("0.1"));</v>
       </c>
     </row>
@@ -1816,7 +1941,7 @@
         <v>0.01</v>
       </c>
       <c r="C3" t="str">
-        <f>"rates.put("""&amp;A3&amp;""",new BigDecimal("""&amp;B3&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("cm-&gt;m",new BigDecimal("0.01"));</v>
       </c>
     </row>
@@ -1828,7 +1953,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="str">
-        <f>"rates.put("""&amp;A4&amp;""",new BigDecimal("""&amp;B4&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("cm-&gt;mm",new BigDecimal("10"));</v>
       </c>
     </row>
@@ -1840,7 +1965,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="str">
-        <f>"rates.put("""&amp;A5&amp;""",new BigDecimal("""&amp;B5&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("dm-&gt;cm",new BigDecimal("10"));</v>
       </c>
     </row>
@@ -1852,7 +1977,7 @@
         <v>0.1</v>
       </c>
       <c r="C6" t="str">
-        <f>"rates.put("""&amp;A6&amp;""",new BigDecimal("""&amp;B6&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("dm-&gt;m",new BigDecimal("0.1"));</v>
       </c>
     </row>
@@ -1864,7 +1989,7 @@
         <v>100</v>
       </c>
       <c r="C7" t="str">
-        <f>"rates.put("""&amp;A7&amp;""",new BigDecimal("""&amp;B7&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("dm-&gt;mm",new BigDecimal("100"));</v>
       </c>
     </row>
@@ -1876,7 +2001,7 @@
         <v>100</v>
       </c>
       <c r="C8" t="str">
-        <f>"rates.put("""&amp;A8&amp;""",new BigDecimal("""&amp;B8&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("m-&gt;cm",new BigDecimal("100"));</v>
       </c>
     </row>
@@ -1888,7 +2013,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="str">
-        <f>"rates.put("""&amp;A9&amp;""",new BigDecimal("""&amp;B9&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("m-&gt;dm",new BigDecimal("10"));</v>
       </c>
     </row>
@@ -1900,7 +2025,7 @@
         <v>1000</v>
       </c>
       <c r="C10" t="str">
-        <f>"rates.put("""&amp;A10&amp;""",new BigDecimal("""&amp;B10&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("m-&gt;mm",new BigDecimal("1000"));</v>
       </c>
     </row>
@@ -1912,7 +2037,7 @@
         <v>0.1</v>
       </c>
       <c r="C11" t="str">
-        <f>"rates.put("""&amp;A11&amp;""",new BigDecimal("""&amp;B11&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("mm-&gt;cm",new BigDecimal("0.1"));</v>
       </c>
     </row>
@@ -1924,7 +2049,7 @@
         <v>0.01</v>
       </c>
       <c r="C12" t="str">
-        <f>"rates.put("""&amp;A12&amp;""",new BigDecimal("""&amp;B12&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("mm-&gt;dm",new BigDecimal("0.01"));</v>
       </c>
     </row>
@@ -1936,7 +2061,7 @@
         <v>1E-3</v>
       </c>
       <c r="C13" t="str">
-        <f>"rates.put("""&amp;A13&amp;""",new BigDecimal("""&amp;B13&amp;"""));"</f>
+        <f t="shared" si="0"/>
         <v>rates.put("mm-&gt;m",new BigDecimal("0.001"));</v>
       </c>
     </row>

</xml_diff>